<commit_message>
new update of SRS document after viewing the review sheet
</commit_message>
<xml_diff>
--- a/Software specification/SRS/SRS_Review.xlsx
+++ b/Software specification/SRS/SRS_Review.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\mina\embeded_systems\ES_ITI_intake_40\Software_engineering\Calculator_repo\Software-Engineering\SWE_Calculator\Software specification\SRS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="945" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="52">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -195,12 +200,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -251,6 +256,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -278,7 +289,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -436,6 +447,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -443,7 +469,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -499,38 +525,41 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -539,103 +568,7 @@
     <cellStyle name="Normal 3 2" xfId="1"/>
     <cellStyle name="Normal 4" xfId="2"/>
   </cellStyles>
-  <dxfs count="70">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="62">
     <dxf>
       <font>
         <condense val="0"/>
@@ -1716,233 +1649,209 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H18"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J24" activeCellId="1" sqref="A8:H8 J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8">
-      <c r="B3" s="28" t="s">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="30" t="s">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-    </row>
-    <row r="4" spans="2:8">
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-    </row>
-    <row r="5" spans="2:8">
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-    </row>
-    <row r="6" spans="2:8">
-      <c r="B6" s="28" t="s">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="24" t="s">
+      <c r="C6" s="21"/>
+      <c r="D6" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-    </row>
-    <row r="7" spans="2:8">
-      <c r="B7" s="28" t="s">
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="31" t="s">
+      <c r="C7" s="21"/>
+      <c r="D7" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-    </row>
-    <row r="8" spans="2:8">
-      <c r="B8" s="28" t="s">
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="24" t="s">
+      <c r="C8" s="21"/>
+      <c r="D8" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-    </row>
-    <row r="9" spans="2:8">
-      <c r="B9" s="28" t="s">
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="24" t="s">
+      <c r="C9" s="21"/>
+      <c r="D9" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-    </row>
-    <row r="10" spans="2:8">
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-    </row>
-    <row r="11" spans="2:8">
-      <c r="B11" s="25" t="s">
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-    </row>
-    <row r="12" spans="2:8">
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26" t="s">
+      <c r="D12" s="27"/>
+      <c r="E12" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="27" t="s">
+      <c r="F12" s="27"/>
+      <c r="G12" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="27"/>
-    </row>
-    <row r="13" spans="2:8">
+      <c r="H12" s="28"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>0.1</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23" t="s">
+      <c r="D13" s="29"/>
+      <c r="E13" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="23"/>
-      <c r="G13" s="24" t="s">
+      <c r="F13" s="29"/>
+      <c r="G13" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="24"/>
-    </row>
-    <row r="14" spans="2:8">
+      <c r="H13" s="23"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-    </row>
-    <row r="15" spans="2:8">
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-    </row>
-    <row r="16" spans="2:8">
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-    </row>
-    <row r="17" spans="2:8">
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-    </row>
-    <row r="18" spans="2:8">
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:H18"/>
@@ -1952,6 +1861,30 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1959,14 +1892,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="D29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="19" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
@@ -1978,7 +1911,7 @@
     <col min="10" max="10" width="174.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="34.15" customHeight="1">
+    <row r="1" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -2001,7 +1934,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="20">
         <v>44014</v>
       </c>
@@ -2024,7 +1957,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <v>44014</v>
       </c>
@@ -2047,7 +1980,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <v>44014</v>
       </c>
@@ -2073,7 +2006,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>44014</v>
       </c>
@@ -2096,7 +2029,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="30">
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <v>44014</v>
       </c>
@@ -2119,7 +2052,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="30">
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>44014</v>
       </c>
@@ -2132,7 +2065,9 @@
       <c r="D7" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="10"/>
+      <c r="E7" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="F7" s="19" t="s">
         <v>25</v>
       </c>
@@ -2146,7 +2081,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>44014</v>
       </c>
@@ -2159,7 +2094,9 @@
       <c r="D8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="10"/>
+      <c r="E8" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="F8" s="19" t="s">
         <v>25</v>
       </c>
@@ -2171,7 +2108,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="45">
+    <row r="9" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20">
         <v>44014</v>
       </c>
@@ -2194,7 +2131,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20">
         <v>44014</v>
       </c>
@@ -2207,13 +2144,15 @@
       <c r="D10" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="F10" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:10" ht="60">
+      <c r="G10" s="32"/>
+    </row>
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>44014</v>
       </c>
@@ -2226,13 +2165,15 @@
       <c r="D11" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="10"/>
+      <c r="E11" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="F11" s="19" t="s">
         <v>25</v>
       </c>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="75">
+    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>44014</v>
       </c>
@@ -2245,13 +2186,15 @@
       <c r="D12" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="10"/>
+      <c r="E12" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="F12" s="19" t="s">
         <v>25</v>
       </c>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>44014</v>
       </c>
@@ -2264,13 +2207,15 @@
       <c r="D13" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="10"/>
+      <c r="E13" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="F13" s="19" t="s">
         <v>25</v>
       </c>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <v>44014</v>
       </c>
@@ -2283,13 +2228,15 @@
       <c r="D14" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="10"/>
+      <c r="E14" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="F14" s="19" t="s">
         <v>25</v>
       </c>
       <c r="G14" s="15"/>
     </row>
-    <row r="15" spans="1:10" ht="30">
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>44014</v>
       </c>
@@ -2302,13 +2249,15 @@
       <c r="D15" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="10"/>
+      <c r="E15" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="F15" s="19" t="s">
         <v>25</v>
       </c>
       <c r="G15" s="15"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>44014</v>
       </c>
@@ -2321,13 +2270,15 @@
       <c r="D16" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="10"/>
+      <c r="E16" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="F16" s="19" t="s">
         <v>25</v>
       </c>
       <c r="G16" s="15"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="12"/>
       <c r="C17" s="13"/>
@@ -2336,7 +2287,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="15"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="13"/>
@@ -2345,7 +2296,7 @@
       <c r="F18" s="10"/>
       <c r="G18" s="15"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="12"/>
       <c r="C19" s="13"/>
@@ -2354,7 +2305,7 @@
       <c r="F19" s="10"/>
       <c r="G19" s="15"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="12"/>
       <c r="C20" s="13"/>
@@ -2363,7 +2314,7 @@
       <c r="F20" s="10"/>
       <c r="G20" s="15"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="12"/>
       <c r="C21" s="13"/>
@@ -2372,7 +2323,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="15"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="12"/>
       <c r="C22" s="13"/>
@@ -2381,7 +2332,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="12"/>
       <c r="C23" s="13"/>
@@ -2390,7 +2341,7 @@
       <c r="F23" s="10"/>
       <c r="G23" s="15"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
@@ -2399,7 +2350,7 @@
       <c r="F24" s="10"/>
       <c r="G24" s="15"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -2408,7 +2359,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="15"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
@@ -2417,7 +2368,7 @@
       <c r="F26" s="10"/>
       <c r="G26" s="15"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -2426,7 +2377,7 @@
       <c r="F27" s="10"/>
       <c r="G27" s="15"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -2435,7 +2386,7 @@
       <c r="F28" s="10"/>
       <c r="G28" s="15"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -2444,7 +2395,7 @@
       <c r="F29" s="10"/>
       <c r="G29" s="15"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -2453,7 +2404,7 @@
       <c r="F30" s="10"/>
       <c r="G30" s="15"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -2462,7 +2413,7 @@
       <c r="F31" s="10"/>
       <c r="G31" s="15"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
@@ -2471,7 +2422,7 @@
       <c r="F32" s="10"/>
       <c r="G32" s="15"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -2480,7 +2431,7 @@
       <c r="F33" s="10"/>
       <c r="G33" s="15"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -2489,7 +2440,7 @@
       <c r="F34" s="10"/>
       <c r="G34" s="15"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -2498,7 +2449,7 @@
       <c r="F35" s="10"/>
       <c r="G35" s="15"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
@@ -2507,7 +2458,7 @@
       <c r="F36" s="10"/>
       <c r="G36" s="15"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
@@ -2516,7 +2467,7 @@
       <c r="F37" s="10"/>
       <c r="G37" s="15"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
@@ -2525,7 +2476,7 @@
       <c r="F38" s="10"/>
       <c r="G38" s="15"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
@@ -2534,7 +2485,7 @@
       <c r="F39" s="10"/>
       <c r="G39" s="15"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
@@ -2543,7 +2494,7 @@
       <c r="F40" s="10"/>
       <c r="G40" s="15"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
@@ -2552,7 +2503,7 @@
       <c r="F41" s="10"/>
       <c r="G41" s="15"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
@@ -2561,7 +2512,7 @@
       <c r="F42" s="10"/>
       <c r="G42" s="15"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
@@ -2572,244 +2523,244 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E2">
-    <cfRule type="cellIs" dxfId="69" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="69" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F12">
-    <cfRule type="cellIs" dxfId="68" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="56" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="57" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E2">
-    <cfRule type="cellIs" dxfId="66" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="70" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="71" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="72" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="73" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="62" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="54" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="55" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F12">
-    <cfRule type="cellIs" dxfId="60" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="53" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="52" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="58" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="51" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="57" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="47" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="48" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="49" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="50" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="53" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="45" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="51" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="44" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="50" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="40" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="41" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="42" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="43" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="46" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="39" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="44" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="37" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="43" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="36" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="39" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="37" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="30" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="36" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="26" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="32" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="cellIs" dxfId="30" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="cellIs" dxfId="28" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="26" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="25" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="21" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2830,6 +2781,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update points 7,12,13,15,16,17,18 Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Software specification/SRS/SRS_Review.xlsx
+++ b/Software specification/SRS/SRS_Review.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\mina\embeded_systems\ES_ITI_intake_40\Software_engineering\Calculator_repo\Software-Engineering\SWE_Calculator\Software specification\SRS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="945" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="500" activeTab="1"/>
   </bookViews>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="56">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -172,9 +167,6 @@
 Don’t display + sign before the operand, no need for that just "- sign" is needed</t>
   </si>
   <si>
-    <t>Ali 13/2/2020: Don't display word "sign", I meant "-" sign</t>
-  </si>
-  <si>
     <t>No need for requirement SRS_006</t>
   </si>
   <si>
@@ -196,16 +188,32 @@
   <si>
     <t xml:space="preserve">There is no differnce between SRS_001 and SRS_002 they have the same scope "detecting the pressed key" </t>
   </si>
+  <si>
+    <t>Ali 19/2/2020: Point is closed</t>
+  </si>
+  <si>
+    <t>19/2/2020</t>
+  </si>
+  <si>
+    <t>In SRS_006 : Inputs shall be "Data, postion"</t>
+  </si>
+  <si>
+    <t>There is many requirements contains the same requirement "SW shall display on LCD the send data on the sent position" hust one requirement about LCD is enough</t>
+  </si>
+  <si>
+    <t>Ali 13/2/2020: Don't display word "sign", I meant "-" sign
+Ali 19/2/2020: Point is closed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -256,12 +264,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -289,7 +291,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -447,21 +449,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -469,7 +456,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -485,9 +472,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -525,19 +509,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -549,17 +530,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -568,7 +561,295 @@
     <cellStyle name="Normal 3 2" xfId="1"/>
     <cellStyle name="Normal 4" xfId="2"/>
   </cellStyles>
-  <dxfs count="62">
+  <dxfs count="86">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -1649,61 +1930,61 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:H18"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J24" activeCellId="1" sqref="A8:H8 J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="21" t="s">
+    <row r="3" spans="2:8">
+      <c r="B3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22" t="s">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="21" t="s">
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="21"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="23" t="s">
         <v>3</v>
       </c>
@@ -1712,24 +1993,24 @@
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="21" t="s">
+    <row r="7" spans="2:8">
+      <c r="B7" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="24" t="s">
+      <c r="C7" s="27"/>
+      <c r="D7" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="21" t="s">
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="21"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="23" t="s">
         <v>7</v>
       </c>
@@ -1738,11 +2019,11 @@
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+    <row r="9" spans="2:8">
+      <c r="B9" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="21"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="23" t="s">
         <v>9</v>
       </c>
@@ -1751,107 +2032,131 @@
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="26" t="s">
+    <row r="10" spans="2:8">
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+    </row>
+    <row r="12" spans="2:8">
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27" t="s">
+      <c r="D12" s="25"/>
+      <c r="E12" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="28" t="s">
+      <c r="F12" s="25"/>
+      <c r="G12" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="28"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H12" s="26"/>
+    </row>
+    <row r="13" spans="2:8">
       <c r="B13" s="2">
         <v>0.1</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29" t="s">
+      <c r="D13" s="22"/>
+      <c r="E13" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="29"/>
+      <c r="F13" s="22"/>
       <c r="G13" s="23" t="s">
         <v>16</v>
       </c>
       <c r="H13" s="23"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8">
       <c r="B14" s="2"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
       <c r="G14" s="23"/>
       <c r="H14" s="23"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8">
       <c r="B15" s="2"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
       <c r="G15" s="23"/>
       <c r="H15" s="23"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8">
       <c r="B16" s="2"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
       <c r="G16" s="23"/>
       <c r="H16" s="23"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8">
       <c r="B17" s="2"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
       <c r="G17" s="23"/>
       <c r="H17" s="23"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8">
       <c r="B18" s="3"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:H18"/>
@@ -1861,30 +2166,6 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1892,16 +2173,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="19" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="18" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="100.42578125" customWidth="1"/>
@@ -1911,7 +2192,7 @@
     <col min="10" max="10" width="174.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="34.15" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -1934,8 +2215,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="20">
+    <row r="2" spans="1:10">
+      <c r="A2" s="19">
         <v>44014</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1944,21 +2225,21 @@
       <c r="C2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="18" t="s">
         <v>42</v>
       </c>
       <c r="G2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="20">
+    <row r="3" spans="1:10">
+      <c r="A3" s="19">
         <v>44014</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -1967,21 +2248,21 @@
       <c r="C3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>42</v>
       </c>
       <c r="G3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="20">
+    <row r="4" spans="1:10">
+      <c r="A4" s="19">
         <v>44014</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -1990,24 +2271,24 @@
       <c r="C4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="31" t="s">
         <v>43</v>
       </c>
       <c r="I4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="20">
+    <row r="5" spans="1:10" ht="30">
+      <c r="A5" s="19">
         <v>44014</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -2016,21 +2297,21 @@
       <c r="C5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="31" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
+    <row r="6" spans="1:10" ht="30">
+      <c r="A6" s="19">
         <v>44014</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -2039,21 +2320,21 @@
       <c r="C6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="31" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="20">
+    <row r="7" spans="1:10" ht="30">
+      <c r="A7" s="19">
         <v>44014</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -2062,17 +2343,17 @@
       <c r="C7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" t="s">
-        <v>45</v>
+      <c r="F7" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>55</v>
       </c>
       <c r="I7" t="s">
         <v>27</v>
@@ -2081,8 +2362,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="20">
+    <row r="8" spans="1:10">
+      <c r="A8" s="19">
         <v>44014</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -2091,16 +2372,16 @@
       <c r="C8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="8"/>
+      <c r="G8" s="32"/>
       <c r="I8" t="s">
         <v>29</v>
       </c>
@@ -2108,8 +2389,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20">
+    <row r="9" spans="1:10" ht="45">
+      <c r="A9" s="19">
         <v>44014</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -2118,21 +2399,21 @@
       <c r="C9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="31" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20">
+    <row r="10" spans="1:10">
+      <c r="A10" s="19">
         <v>44014</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -2141,19 +2422,19 @@
       <c r="C10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="18" t="s">
         <v>25</v>
       </c>
       <c r="G10" s="32"/>
     </row>
-    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="20">
+    <row r="11" spans="1:10" ht="60">
+      <c r="A11" s="19">
         <v>44014</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -2162,19 +2443,19 @@
       <c r="C11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="10" t="s">
+      <c r="D11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="20">
+      <c r="G11" s="32"/>
+    </row>
+    <row r="12" spans="1:10" ht="75">
+      <c r="A12" s="19">
         <v>44014</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -2183,600 +2464,676 @@
       <c r="C12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="15"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="20">
+      <c r="F12" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="19">
         <v>44014</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="15"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="20">
+      <c r="F13" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="19">
         <v>44014</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="15"/>
-    </row>
-    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="20">
+      <c r="G14" s="33"/>
+    </row>
+    <row r="15" spans="1:10" ht="30">
+      <c r="A15" s="19">
         <v>44014</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="15"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="20">
+      <c r="F15" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="19">
         <v>44014</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="19" t="s">
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="15"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="15"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="15"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="15"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="15"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="15"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="15"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="15"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="15"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="15"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="15"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="15"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="15"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="15"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="15"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="15"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="15"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="15"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="15"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="15"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="15"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="15"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="15"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="15"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="15"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="15"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="15"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="15"/>
+      <c r="G17" s="31"/>
+    </row>
+    <row r="18" spans="1:7" ht="25.5">
+      <c r="A18" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="14"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="14"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="14"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="10"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="14"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="10"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="14"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="10"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="14"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="14"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="14"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="10"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="14"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="14"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="14"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="14"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="14"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="14"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="14"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="14"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="14"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="14"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="14"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="14"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="14"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="14"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E2">
-    <cfRule type="cellIs" dxfId="61" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="81" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F12">
-    <cfRule type="cellIs" dxfId="60" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="68" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="69" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E2">
-    <cfRule type="cellIs" dxfId="58" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="82" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="83" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="84" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="85" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="54" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="66" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="67" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F12">
-    <cfRule type="cellIs" dxfId="52" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="65" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="64" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="50" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="63" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="49" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="59" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="60" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="61" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="62" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="45" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="57" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="58" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="43" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="56" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="42" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="52" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="53" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="54" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="55" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="50" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="51" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="36" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="49" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="45" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="46" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="47" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="48" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="43" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="44" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="29" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="42" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="28" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="38" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="39" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="40" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="41" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="36" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="37" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="34" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="35" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="32" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="33" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="31" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="27" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="28" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="29" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="30" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="25" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="26" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="23" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="24" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="21" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="22" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="19" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="20" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="17" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="18" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="15" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="16" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="14" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F15">
+    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 E17:E1043">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 E19:E1043">
       <formula1>$I$4:$I$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1 F17:F1043">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1 F19:F1043">
       <formula1>#REF!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E18">
       <formula1>"Refused, Accepted"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F18">
       <formula1>"Open, Resolved"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated SRS after review and adding Context Diagram
</commit_message>
<xml_diff>
--- a/Software specification/SRS/SRS_Review.xlsx
+++ b/Software specification/SRS/SRS_Review.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\mina\embeded_systems\ES_ITI_intake_40\Software_engineering\Calculator_repo\Software-Engineering\SWE_Calculator\Software specification\SRS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1890" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="56">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -208,12 +213,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -509,39 +514,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -554,6 +526,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Accent3" xfId="3"/>
@@ -561,151 +566,7 @@
     <cellStyle name="Normal 3 2" xfId="1"/>
     <cellStyle name="Normal 4" xfId="2"/>
   </cellStyles>
-  <dxfs count="86">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="74">
     <dxf>
       <font>
         <condense val="0"/>
@@ -1930,109 +1791,109 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H18"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J24" activeCellId="1" sqref="A8:H8 J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8">
-      <c r="B3" s="27" t="s">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="29" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-    </row>
-    <row r="4" spans="2:8">
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-    </row>
-    <row r="5" spans="2:8">
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-    </row>
-    <row r="6" spans="2:8">
-      <c r="B6" s="27" t="s">
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="23" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-    </row>
-    <row r="7" spans="2:8">
-      <c r="B7" s="27" t="s">
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="30" t="s">
+      <c r="C7" s="24"/>
+      <c r="D7" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-    </row>
-    <row r="8" spans="2:8">
-      <c r="B8" s="27" t="s">
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="23" t="s">
+      <c r="C8" s="24"/>
+      <c r="D8" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-    </row>
-    <row r="9" spans="2:8">
-      <c r="B9" s="27" t="s">
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="23" t="s">
+      <c r="C9" s="24"/>
+      <c r="D9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-    </row>
-    <row r="10" spans="2:8">
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="28"/>
       <c r="C10" s="28"/>
       <c r="D10" s="28"/>
@@ -2041,122 +1902,98 @@
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
     </row>
-    <row r="11" spans="2:8">
-      <c r="B11" s="24" t="s">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-    </row>
-    <row r="12" spans="2:8">
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25" t="s">
+      <c r="D12" s="30"/>
+      <c r="E12" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="26" t="s">
+      <c r="F12" s="30"/>
+      <c r="G12" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="26"/>
-    </row>
-    <row r="13" spans="2:8">
+      <c r="H12" s="31"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>0.1</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22" t="s">
+      <c r="D13" s="32"/>
+      <c r="E13" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="22"/>
-      <c r="G13" s="23" t="s">
+      <c r="F13" s="32"/>
+      <c r="G13" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="23"/>
-    </row>
-    <row r="14" spans="2:8">
+      <c r="H13" s="26"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-    </row>
-    <row r="15" spans="2:8">
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-    </row>
-    <row r="16" spans="2:8">
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-    </row>
-    <row r="17" spans="2:8">
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-    </row>
-    <row r="18" spans="2:8">
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:H18"/>
@@ -2166,6 +2003,30 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2173,14 +2034,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="B15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="18" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
@@ -2192,7 +2053,7 @@
     <col min="10" max="10" width="174.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="34.15" customHeight="1">
+    <row r="1" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -2215,7 +2076,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="19">
         <v>44014</v>
       </c>
@@ -2238,7 +2099,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="19">
         <v>44014</v>
       </c>
@@ -2261,7 +2122,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
         <v>44014</v>
       </c>
@@ -2280,14 +2141,14 @@
       <c r="F4" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="20" t="s">
         <v>43</v>
       </c>
       <c r="I4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>44014</v>
       </c>
@@ -2306,11 +2167,11 @@
       <c r="F5" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="30">
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>44014</v>
       </c>
@@ -2329,11 +2190,11 @@
       <c r="F6" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="G6" s="20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="30">
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>44014</v>
       </c>
@@ -2352,7 +2213,7 @@
       <c r="F7" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="23" t="s">
         <v>55</v>
       </c>
       <c r="I7" t="s">
@@ -2362,7 +2223,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>44014</v>
       </c>
@@ -2381,7 +2242,7 @@
       <c r="F8" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="32"/>
+      <c r="G8" s="21"/>
       <c r="I8" t="s">
         <v>29</v>
       </c>
@@ -2389,7 +2250,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="45">
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>44014</v>
       </c>
@@ -2408,11 +2269,11 @@
       <c r="F9" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>44014</v>
       </c>
@@ -2431,9 +2292,9 @@
       <c r="F10" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="32"/>
-    </row>
-    <row r="11" spans="1:10" ht="60">
+      <c r="G10" s="21"/>
+    </row>
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>44014</v>
       </c>
@@ -2452,9 +2313,9 @@
       <c r="F11" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="32"/>
-    </row>
-    <row r="12" spans="1:10" ht="75">
+      <c r="G11" s="21"/>
+    </row>
+    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>44014</v>
       </c>
@@ -2473,11 +2334,11 @@
       <c r="F12" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="G12" s="20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>44014</v>
       </c>
@@ -2496,11 +2357,11 @@
       <c r="F13" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="G13" s="20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>44014</v>
       </c>
@@ -2519,9 +2380,9 @@
       <c r="F14" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="33"/>
-    </row>
-    <row r="15" spans="1:10" ht="30">
+      <c r="G14" s="22"/>
+    </row>
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>44014</v>
       </c>
@@ -2540,11 +2401,11 @@
       <c r="F15" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>44014</v>
       </c>
@@ -2563,11 +2424,11 @@
       <c r="F16" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="31" t="s">
+      <c r="G16" s="20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>52</v>
       </c>
@@ -2580,13 +2441,15 @@
       <c r="D17" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="9"/>
+      <c r="E17" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="F17" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="31"/>
-    </row>
-    <row r="18" spans="1:7" ht="25.5">
+      <c r="G17" s="20"/>
+    </row>
+    <row r="18" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>52</v>
       </c>
@@ -2599,13 +2462,15 @@
       <c r="D18" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="9"/>
+      <c r="E18" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="F18" s="18" t="s">
         <v>25</v>
       </c>
       <c r="G18" s="14"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="12"/>
@@ -2614,7 +2479,7 @@
       <c r="F19" s="9"/>
       <c r="G19" s="14"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="11"/>
       <c r="C20" s="12"/>
@@ -2623,7 +2488,7 @@
       <c r="F20" s="9"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="C21" s="12"/>
@@ -2632,7 +2497,7 @@
       <c r="F21" s="9"/>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
@@ -2641,7 +2506,7 @@
       <c r="F22" s="9"/>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
@@ -2650,7 +2515,7 @@
       <c r="F23" s="9"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -2659,7 +2524,7 @@
       <c r="F24" s="9"/>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -2668,7 +2533,7 @@
       <c r="F25" s="9"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -2677,7 +2542,7 @@
       <c r="F26" s="9"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -2686,7 +2551,7 @@
       <c r="F27" s="9"/>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -2695,7 +2560,7 @@
       <c r="F28" s="9"/>
       <c r="G28" s="14"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -2704,7 +2569,7 @@
       <c r="F29" s="9"/>
       <c r="G29" s="14"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -2713,7 +2578,7 @@
       <c r="F30" s="9"/>
       <c r="G30" s="14"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
@@ -2722,7 +2587,7 @@
       <c r="F31" s="9"/>
       <c r="G31" s="14"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -2731,7 +2596,7 @@
       <c r="F32" s="9"/>
       <c r="G32" s="14"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
@@ -2740,7 +2605,7 @@
       <c r="F33" s="9"/>
       <c r="G33" s="14"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
@@ -2749,7 +2614,7 @@
       <c r="F34" s="9"/>
       <c r="G34" s="14"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
@@ -2758,7 +2623,7 @@
       <c r="F35" s="9"/>
       <c r="G35" s="14"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
@@ -2767,7 +2632,7 @@
       <c r="F36" s="9"/>
       <c r="G36" s="14"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
@@ -2776,7 +2641,7 @@
       <c r="F37" s="9"/>
       <c r="G37" s="14"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
@@ -2785,7 +2650,7 @@
       <c r="F38" s="9"/>
       <c r="G38" s="14"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
@@ -2794,7 +2659,7 @@
       <c r="F39" s="9"/>
       <c r="G39" s="14"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
@@ -2803,7 +2668,7 @@
       <c r="F40" s="9"/>
       <c r="G40" s="14"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
@@ -2812,7 +2677,7 @@
       <c r="F41" s="9"/>
       <c r="G41" s="14"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
@@ -2821,7 +2686,7 @@
       <c r="F42" s="9"/>
       <c r="G42" s="14"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
@@ -2832,292 +2697,292 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E2">
-    <cfRule type="cellIs" dxfId="85" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="81" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F12">
-    <cfRule type="cellIs" dxfId="84" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="68" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="69" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E2">
-    <cfRule type="cellIs" dxfId="82" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="82" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="83" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="84" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="85" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="78" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="66" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="67" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F12">
-    <cfRule type="cellIs" dxfId="76" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="65" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="64" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="74" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="63" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="73" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="59" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="60" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="61" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="62" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="69" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="57" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="58" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="67" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="56" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="66" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="52" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="53" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="54" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="55" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="62" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="50" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="51" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="60" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="49" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="59" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="45" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="55" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="43" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="44" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="53" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="42" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="52" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="38" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="39" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="41" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="48" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="36" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="cellIs" dxfId="46" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="cellIs" dxfId="44" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="42" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="31" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="41" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="27" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="37" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="cellIs" dxfId="35" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="cellIs" dxfId="33" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="31" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="29" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="27" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17">
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update SRS after review
</commit_message>
<xml_diff>
--- a/Software specification/SRS/SRS_Review.xlsx
+++ b/Software specification/SRS/SRS_Review.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\mina\embeded_systems\ES_ITI_intake_40\Software_engineering\Calculator_repo\Software-Engineering\SWE_Calculator\Software specification\SRS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2835" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="61">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -223,12 +228,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -536,16 +541,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -557,16 +565,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -576,7 +581,7 @@
     <cellStyle name="Normal 3 2" xfId="1"/>
     <cellStyle name="Normal 4" xfId="2"/>
   </cellStyles>
-  <dxfs count="102">
+  <dxfs count="86">
     <dxf>
       <font>
         <condense val="0"/>
@@ -694,198 +699,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2137,233 +1950,209 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H18"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J24" activeCellId="1" sqref="A8:H8 J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8">
-      <c r="B3" s="31" t="s">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="33" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-    </row>
-    <row r="4" spans="2:8">
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-    </row>
-    <row r="5" spans="2:8">
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-    </row>
-    <row r="6" spans="2:8">
-      <c r="B6" s="31" t="s">
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="27" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-    </row>
-    <row r="7" spans="2:8">
-      <c r="B7" s="31" t="s">
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="34" t="s">
+      <c r="C7" s="24"/>
+      <c r="D7" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-    </row>
-    <row r="8" spans="2:8">
-      <c r="B8" s="31" t="s">
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="27" t="s">
+      <c r="C8" s="24"/>
+      <c r="D8" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-    </row>
-    <row r="9" spans="2:8">
-      <c r="B9" s="31" t="s">
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="27" t="s">
+      <c r="C9" s="24"/>
+      <c r="D9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-    </row>
-    <row r="10" spans="2:8">
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-    </row>
-    <row r="11" spans="2:8">
-      <c r="B11" s="28" t="s">
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-    </row>
-    <row r="12" spans="2:8">
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29" t="s">
+      <c r="D12" s="30"/>
+      <c r="E12" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="29"/>
-      <c r="G12" s="30" t="s">
+      <c r="F12" s="30"/>
+      <c r="G12" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="30"/>
-    </row>
-    <row r="13" spans="2:8">
+      <c r="H12" s="31"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>0.1</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26" t="s">
+      <c r="D13" s="32"/>
+      <c r="E13" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="26"/>
-      <c r="G13" s="27" t="s">
+      <c r="F13" s="32"/>
+      <c r="G13" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="27"/>
-    </row>
-    <row r="14" spans="2:8">
+      <c r="H13" s="26"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-    </row>
-    <row r="15" spans="2:8">
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-    </row>
-    <row r="16" spans="2:8">
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-    </row>
-    <row r="17" spans="2:8">
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-    </row>
-    <row r="18" spans="2:8">
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:H18"/>
@@ -2373,6 +2162,30 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2380,14 +2193,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="18" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
@@ -2399,7 +2212,7 @@
     <col min="10" max="10" width="174.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="34.15" customHeight="1">
+    <row r="1" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -2422,7 +2235,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="19">
         <v>44014</v>
       </c>
@@ -2445,7 +2258,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="19">
         <v>44014</v>
       </c>
@@ -2468,7 +2281,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
         <v>44014</v>
       </c>
@@ -2494,7 +2307,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>44014</v>
       </c>
@@ -2517,7 +2330,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="30">
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>44014</v>
       </c>
@@ -2540,7 +2353,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="30">
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>44014</v>
       </c>
@@ -2569,7 +2382,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>44014</v>
       </c>
@@ -2598,7 +2411,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="45">
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>44014</v>
       </c>
@@ -2621,7 +2434,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>44014</v>
       </c>
@@ -2644,7 +2457,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="60">
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>44014</v>
       </c>
@@ -2667,7 +2480,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="75">
+    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>44014</v>
       </c>
@@ -2690,7 +2503,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>44014</v>
       </c>
@@ -2713,7 +2526,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>44014</v>
       </c>
@@ -2734,7 +2547,7 @@
       </c>
       <c r="G14" s="22"/>
     </row>
-    <row r="15" spans="1:10" ht="30">
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>44014</v>
       </c>
@@ -2757,7 +2570,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>44014</v>
       </c>
@@ -2780,7 +2593,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>52</v>
       </c>
@@ -2801,7 +2614,7 @@
       </c>
       <c r="G17" s="20"/>
     </row>
-    <row r="18" spans="1:7" ht="25.5">
+    <row r="18" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>52</v>
       </c>
@@ -2822,7 +2635,7 @@
       </c>
       <c r="G18" s="14"/>
     </row>
-    <row r="19" spans="1:7" ht="25.5">
+    <row r="19" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>52</v>
       </c>
@@ -2835,13 +2648,15 @@
       <c r="D19" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="9"/>
+      <c r="E19" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="F19" s="18" t="s">
         <v>25</v>
       </c>
       <c r="G19" s="14"/>
     </row>
-    <row r="20" spans="1:7" ht="25.5">
+    <row r="20" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>52</v>
       </c>
@@ -2854,13 +2669,15 @@
       <c r="D20" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="9"/>
+      <c r="E20" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="F20" s="18" t="s">
         <v>25</v>
       </c>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>52</v>
       </c>
@@ -2873,13 +2690,15 @@
       <c r="D21" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E21" s="9"/>
+      <c r="E21" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="F21" s="18" t="s">
         <v>25</v>
       </c>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
@@ -2888,7 +2707,7 @@
       <c r="F22" s="9"/>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
@@ -2897,7 +2716,7 @@
       <c r="F23" s="9"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -2906,7 +2725,7 @@
       <c r="F24" s="9"/>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -2915,7 +2734,7 @@
       <c r="F25" s="9"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -2924,7 +2743,7 @@
       <c r="F26" s="9"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -2933,7 +2752,7 @@
       <c r="F27" s="9"/>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -2942,7 +2761,7 @@
       <c r="F28" s="9"/>
       <c r="G28" s="14"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -2951,7 +2770,7 @@
       <c r="F29" s="9"/>
       <c r="G29" s="14"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -2960,7 +2779,7 @@
       <c r="F30" s="9"/>
       <c r="G30" s="14"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
@@ -2969,7 +2788,7 @@
       <c r="F31" s="9"/>
       <c r="G31" s="14"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -2978,7 +2797,7 @@
       <c r="F32" s="9"/>
       <c r="G32" s="14"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
@@ -2987,7 +2806,7 @@
       <c r="F33" s="9"/>
       <c r="G33" s="14"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
@@ -2996,7 +2815,7 @@
       <c r="F34" s="9"/>
       <c r="G34" s="14"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
@@ -3005,7 +2824,7 @@
       <c r="F35" s="9"/>
       <c r="G35" s="14"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
@@ -3014,7 +2833,7 @@
       <c r="F36" s="9"/>
       <c r="G36" s="14"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
@@ -3023,7 +2842,7 @@
       <c r="F37" s="9"/>
       <c r="G37" s="14"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
@@ -3032,7 +2851,7 @@
       <c r="F38" s="9"/>
       <c r="G38" s="14"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
@@ -3041,7 +2860,7 @@
       <c r="F39" s="9"/>
       <c r="G39" s="14"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
@@ -3050,7 +2869,7 @@
       <c r="F40" s="9"/>
       <c r="G40" s="14"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
@@ -3059,7 +2878,7 @@
       <c r="F41" s="9"/>
       <c r="G41" s="14"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
@@ -3068,7 +2887,7 @@
       <c r="F42" s="9"/>
       <c r="G42" s="14"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
@@ -3079,340 +2898,340 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E2">
-    <cfRule type="cellIs" dxfId="101" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="93" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F12">
-    <cfRule type="cellIs" dxfId="100" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="80" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="81" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E2">
-    <cfRule type="cellIs" dxfId="98" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="94" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="95" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="96" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="97" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="94" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="78" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="79" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F12">
-    <cfRule type="cellIs" dxfId="92" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="77" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="76" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="90" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="75" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="89" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="71" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="72" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="73" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="74" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="85" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="69" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="70" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="83" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="68" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="82" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="64" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="65" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="66" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="67" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="78" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="62" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="63" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="76" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="61" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="75" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="57" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="58" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="59" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="60" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="71" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="55" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="56" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="69" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="54" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="68" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="50" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="51" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="53" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="64" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="48" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="49" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="cellIs" dxfId="62" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="cellIs" dxfId="60" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="44" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="45" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="58" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="43" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="57" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="39" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="40" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="41" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="42" operator="equal">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="53" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="37" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="38" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="cellIs" dxfId="51" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="cellIs" dxfId="49" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="47" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="45" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="43" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="41" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="39" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="37" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17">
-    <cfRule type="cellIs" dxfId="35" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17">
-    <cfRule type="cellIs" dxfId="33" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="31" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="29" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Review Switch & Buzzer CDDs and update GDD/SRS review Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Software specification/SRS/SRS_Review.xlsx
+++ b/Software specification/SRS/SRS_Review.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\mina\embeded_systems\ES_ITI_intake_40\Software_engineering\Calculator_repo\Software-Engineering\SWE_Calculator\Software specification\SRS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="2835" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="500" activeTab="1"/>
   </bookViews>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="60">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -103,9 +98,6 @@
   </si>
   <si>
     <t xml:space="preserve">Initial Version </t>
-  </si>
-  <si>
-    <t>Open</t>
   </si>
   <si>
     <t>Refused</t>
@@ -228,12 +220,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -541,19 +533,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -565,13 +554,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1950,209 +1942,233 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:H18"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J24" activeCellId="1" sqref="A8:H8 J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
+    <row r="3" spans="2:8">
+      <c r="B3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="24" t="s">
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="26" t="s">
+      <c r="C6" s="31"/>
+      <c r="D6" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="24" t="s">
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="27" t="s">
+      <c r="C7" s="31"/>
+      <c r="D7" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="24" t="s">
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="26" t="s">
+      <c r="C8" s="31"/>
+      <c r="D8" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="24" t="s">
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="26" t="s">
+      <c r="C9" s="31"/>
+      <c r="D9" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="29" t="s">
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+    </row>
+    <row r="12" spans="2:8">
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30" t="s">
+      <c r="D12" s="29"/>
+      <c r="E12" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="30"/>
-      <c r="G12" s="31" t="s">
+      <c r="F12" s="29"/>
+      <c r="G12" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="31"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H12" s="30"/>
+    </row>
+    <row r="13" spans="2:8">
       <c r="B13" s="2">
         <v>0.1</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32" t="s">
+      <c r="D13" s="26"/>
+      <c r="E13" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="26" t="s">
+      <c r="F13" s="26"/>
+      <c r="G13" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="26"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H13" s="27"/>
+    </row>
+    <row r="14" spans="2:8">
       <c r="B14" s="2"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+    </row>
+    <row r="15" spans="2:8">
       <c r="B15" s="2"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+    </row>
+    <row r="16" spans="2:8">
       <c r="B16" s="2"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+    </row>
+    <row r="17" spans="2:8">
       <c r="B17" s="2"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+    </row>
+    <row r="18" spans="2:8">
       <c r="B18" s="3"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:H18"/>
@@ -2162,30 +2178,6 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2193,14 +2185,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="18" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
@@ -2212,7 +2204,7 @@
     <col min="10" max="10" width="174.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="34.15" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -2235,470 +2227,470 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="19">
         <v>44014</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="G2" t="s">
         <v>42</v>
       </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="19">
         <v>44014</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="G3" t="s">
         <v>42</v>
       </c>
-      <c r="G3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="19">
         <v>44014</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="G4" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="20" t="s">
-        <v>43</v>
-      </c>
       <c r="I4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30">
       <c r="A5" s="19">
         <v>44014</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="G5" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" ht="30">
       <c r="A6" s="19">
         <v>44014</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="G6" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" ht="30">
       <c r="A7" s="19">
         <v>44014</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="18" t="s">
-        <v>42</v>
-      </c>
       <c r="G7" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" t="s">
         <v>27</v>
       </c>
-      <c r="J7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="19">
         <v>44014</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="18" t="s">
-        <v>42</v>
-      </c>
       <c r="G8" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" t="s">
         <v>29</v>
       </c>
-      <c r="J8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" ht="45">
       <c r="A9" s="19">
         <v>44014</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="19">
         <v>44014</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="18" t="s">
-        <v>42</v>
-      </c>
       <c r="G10" s="20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="60">
       <c r="A11" s="19">
         <v>44014</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="18" t="s">
-        <v>42</v>
-      </c>
       <c r="G11" s="20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="75">
       <c r="A12" s="19">
         <v>44014</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="18" t="s">
-        <v>42</v>
-      </c>
       <c r="G12" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="19">
         <v>44014</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="18" t="s">
-        <v>42</v>
-      </c>
       <c r="G13" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="19">
         <v>44014</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>48</v>
-      </c>
       <c r="E14" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="18" t="s">
-        <v>25</v>
-      </c>
       <c r="G14" s="22"/>
     </row>
-    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="30">
       <c r="A15" s="19">
         <v>44014</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E15" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>42</v>
-      </c>
       <c r="G15" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="19">
         <v>44014</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D16" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="9" t="s">
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="20" t="s">
+      <c r="G17" s="20"/>
+    </row>
+    <row r="18" spans="1:7" ht="25.5">
+      <c r="A18" s="19" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="13" t="s">
+      <c r="B18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E18" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="20"/>
-    </row>
-    <row r="18" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="9" t="s">
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="1:7" ht="25.5">
+      <c r="A19" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="14"/>
-    </row>
-    <row r="19" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="15" t="s">
+      <c r="G19" s="14"/>
+    </row>
+    <row r="20" spans="1:7" ht="25.5">
+      <c r="A20" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E20" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="14"/>
-    </row>
-    <row r="20" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="15" t="s">
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E21" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="14"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>25</v>
-      </c>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
@@ -2707,7 +2699,7 @@
       <c r="F22" s="9"/>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
@@ -2716,7 +2708,7 @@
       <c r="F23" s="9"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -2725,7 +2717,7 @@
       <c r="F24" s="9"/>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="10"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -2734,7 +2726,7 @@
       <c r="F25" s="9"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -2743,7 +2735,7 @@
       <c r="F26" s="9"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -2752,7 +2744,7 @@
       <c r="F27" s="9"/>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -2761,7 +2753,7 @@
       <c r="F28" s="9"/>
       <c r="G28" s="14"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -2770,7 +2762,7 @@
       <c r="F29" s="9"/>
       <c r="G29" s="14"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -2779,7 +2771,7 @@
       <c r="F30" s="9"/>
       <c r="G30" s="14"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="12"/>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
@@ -2788,7 +2780,7 @@
       <c r="F31" s="9"/>
       <c r="G31" s="14"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -2797,7 +2789,7 @@
       <c r="F32" s="9"/>
       <c r="G32" s="14"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="12"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
@@ -2806,7 +2798,7 @@
       <c r="F33" s="9"/>
       <c r="G33" s="14"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="12"/>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
@@ -2815,7 +2807,7 @@
       <c r="F34" s="9"/>
       <c r="G34" s="14"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" s="12"/>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
@@ -2824,7 +2816,7 @@
       <c r="F35" s="9"/>
       <c r="G35" s="14"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" s="12"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
@@ -2833,7 +2825,7 @@
       <c r="F36" s="9"/>
       <c r="G36" s="14"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
@@ -2842,7 +2834,7 @@
       <c r="F37" s="9"/>
       <c r="G37" s="14"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" s="12"/>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
@@ -2851,7 +2843,7 @@
       <c r="F38" s="9"/>
       <c r="G38" s="14"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" s="12"/>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
@@ -2860,7 +2852,7 @@
       <c r="F39" s="9"/>
       <c r="G39" s="14"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7">
       <c r="A40" s="12"/>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
@@ -2869,7 +2861,7 @@
       <c r="F40" s="9"/>
       <c r="G40" s="14"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" s="12"/>
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
@@ -2878,7 +2870,7 @@
       <c r="F41" s="9"/>
       <c r="G41" s="14"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7">
       <c r="A42" s="12"/>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
@@ -2887,7 +2879,7 @@
       <c r="F42" s="9"/>
       <c r="G42" s="14"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>

</xml_diff>